<commit_message>
Added Model classes for TextAdventureGame
Added the Hazard, Player, PlayerStatus, and Action class to handle business logic. Created tests for all classes.
</commit_message>
<xml_diff>
--- a/documentation/Sprint Backlog  Burndown.xlsx
+++ b/documentation/Sprint Backlog  Burndown.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ja00150\Desktop\TextAdventureGame\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B1B9F8B-7A73-4C69-886E-C06B52EA1787}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B61C6F6-8FDB-4224-AE2F-DAF905F1513A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3075" yWindow="3075" windowWidth="16200" windowHeight="9360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1346,7 +1346,7 @@
   <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1430,7 +1430,9 @@
       <c r="C5" s="1">
         <v>0.5</v>
       </c>
-      <c r="D5" s="2"/>
+      <c r="D5" s="2">
+        <v>0</v>
+      </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
@@ -1443,7 +1445,9 @@
       <c r="C6" s="1">
         <v>2</v>
       </c>
-      <c r="D6" s="2"/>
+      <c r="D6" s="2">
+        <v>0</v>
+      </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -1456,7 +1460,9 @@
       <c r="C7" s="1">
         <v>4</v>
       </c>
-      <c r="D7" s="2"/>
+      <c r="D7" s="2">
+        <v>0</v>
+      </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>

</xml_diff>